<commit_message>
EPBDS-5891 Fix .xlsx to prevent parsing error in POI
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/datatype/WrongAliasDatatype1Test.xlsx
+++ b/DEV/org.openl.rules/test/rules/datatype/WrongAliasDatatype1Test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="270" windowWidth="24495" windowHeight="11700"/>
@@ -27,19 +27,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -53,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -100,24 +92,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -196,6 +204,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -230,6 +239,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -405,65 +415,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
-      <c r="B4" s="2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <v>40179</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
-      <c r="B5" s="3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>0.88</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>